<commit_message>
Add missing participants answers and analyze answers from study 1
</commit_message>
<xml_diff>
--- a/Antworten_Studie1.xlsx
+++ b/Antworten_Studie1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael_M\Documents\GitHub\BA_Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851CF39E-BC24-4A8A-9214-E3DFA1367D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9ABE50-4A27-4293-BD63-1251870C1D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Proband</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Performance/Responsiveness sehr wichtig; deshalb OSM; wäre die Performance besser, dann vermutlich die andere</t>
   </si>
   <si>
-    <t>Haus am See viel besser; Arbeit viel weniger beim Suchen; Orte und Gebiete wechsel sehr hilfreich; Gesamteindruck, vor allem optisch, besser</t>
-  </si>
-  <si>
     <t>bei OSM fast immer relativ unsicher, weil selber messen nötig; bei Haus am See glaubenswürdiger, durch die Filter kann man auch leichter selber nochmal nachschauen</t>
   </si>
   <si>
@@ -166,7 +163,31 @@
     <t>beide nicht allzu gut, lieber Google Maps</t>
   </si>
   <si>
-    <t>für den Anfang sehr gut; aber gerade wenn mit jemand anderem zusammen gesucht hilfreich; aber leider ewig geladen</t>
+    <t>Nutzung im Alltag</t>
+  </si>
+  <si>
+    <t>Haus am see</t>
+  </si>
+  <si>
+    <t>OSM</t>
+  </si>
+  <si>
+    <t>für den Anfang sehr gut; aber gerade wenn mit jemand anderem zusammen sucht sehr hilfreich; aber leider ewig geladen</t>
+  </si>
+  <si>
+    <t>Haus am See viel besser; Arbeit war viel weniger beim Suchen; Orte und Gebiete wechsel sehr hilfreich; Gesamteindruck, vor allem optisch, besser</t>
+  </si>
+  <si>
+    <t>Haus am See / OSM</t>
+  </si>
+  <si>
+    <t>beides schlecht</t>
+  </si>
+  <si>
+    <t>beides gleich</t>
+  </si>
+  <si>
+    <t>keines der beiden</t>
   </si>
 </sst>
 </file>
@@ -210,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -225,11 +246,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -240,6 +302,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E221BB-A872-4BDC-96BF-936F8260F363}" name="Tabelle1" displayName="Tabelle1" ref="J1:M9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="J1:M9" xr:uid="{FC7400E0-BE2B-4C03-BE68-7E071BF25475}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A4E3DB00-EB26-4D01-9606-5266D0C4C0B3}" name="Besser zurechtgekommen" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9CB4B4FC-D4E5-440A-837D-85993AE789E7}" name="Zufriedenheit" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8EE89277-8220-41CC-84C0-7D52C8B07CB3}" name="Intuitivität" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{BD49C7E5-3AEE-4000-92A6-6722459B4289}" name="Nutzung im Alltag" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,9 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -517,9 +599,13 @@
     <col min="4" max="4" width="20.6328125" customWidth="1"/>
     <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="14.1796875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="17.54296875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -539,8 +625,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
+      <c r="J1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -559,8 +658,20 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -579,88 +690,148 @@
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
+      <c r="J6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -679,29 +850,56 @@
       <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
+      <c r="J9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>